<commit_message>
Final commit, fixed silkscreen labels
</commit_message>
<xml_diff>
--- a/EECS430W24_Group7_PCB_BOM.xlsx
+++ b/EECS430W24_Group7_PCB_BOM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Desktop\UMich\Class Files\9 2024 Winter\EECS 430\Project\eecs430-phased-array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7B7A4C-0493-42CB-9528-2C077C75545B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE9A480-B7E1-4A82-8830-10CBCCFF3547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Full BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Condensed BOM" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="143">
   <si>
     <t>Quantity</t>
   </si>
@@ -227,9 +228,6 @@
     <t>https://www.digikey.com/en/products/detail/analog-devices-inc/hmc407ms8getr/3452254</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/psemi/pe42423b-z/4807898</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -278,9 +276,6 @@
     <t>Line Cost</t>
   </si>
   <si>
-    <t>C6,</t>
-  </si>
-  <si>
     <t xml:space="preserve"> C13.1, C13.2, C14.1, C14.2, C17.1, C17.2, C18.1, C18.2</t>
   </si>
   <si>
@@ -423,6 +418,54 @@
   </si>
   <si>
     <t>Per array</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/pSemi/PE42423B-Z?qs=Cb2nCFKsA8oZ1mNDB1JweA%3D%3D</t>
+  </si>
+  <si>
+    <t>Populated</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>SMA Connectors</t>
+  </si>
+  <si>
+    <t>Power Connectors</t>
+  </si>
+  <si>
+    <t>Raspberry PI Connectors</t>
+  </si>
+  <si>
+    <t>Power Amplifier</t>
+  </si>
+  <si>
+    <t>RF Switch</t>
+  </si>
+  <si>
+    <t>Low Noise Amplifier</t>
+  </si>
+  <si>
+    <t>Phase Shifters</t>
+  </si>
+  <si>
+    <t>Miscellaneous Passive Components</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Components</t>
   </si>
 </sst>
 </file>
@@ -779,28 +822,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>57</v>
@@ -815,19 +859,22 @@
         <v>58</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>59</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>5000</v>
       </c>
@@ -844,7 +891,7 @@
         <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>60</v>
@@ -857,12 +904,12 @@
         <v>8.74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -871,13 +918,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H3" s="1">
         <v>1.08</v>
@@ -887,12 +934,12 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -901,13 +948,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H4" s="1">
         <v>1.23</v>
@@ -917,9 +964,9 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -931,13 +978,13 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="H5" s="1">
         <v>3.99</v>
@@ -947,7 +994,7 @@
         <v>11.97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -961,13 +1008,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6" s="1">
         <v>0.75</v>
@@ -977,27 +1024,27 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
         <v>100</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" t="s">
-        <v>102</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H7" s="1">
         <v>2.95</v>
@@ -1007,9 +1054,9 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -1021,13 +1068,13 @@
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H8" s="1">
         <v>0.39</v>
@@ -1036,13 +1083,16 @@
         <f t="shared" si="0"/>
         <v>1.56</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1054,10 +1104,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H9" s="1">
         <v>0.1</v>
@@ -1066,13 +1116,16 @@
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1084,10 +1137,10 @@
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H10" s="1">
         <v>0.11</v>
@@ -1096,8 +1149,11 @@
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -1114,10 +1170,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" s="1">
         <v>0.33</v>
@@ -1126,8 +1182,11 @@
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -1144,10 +1203,10 @@
         <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H12" s="1">
         <v>1.18</v>
@@ -1157,7 +1216,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1174,10 +1233,10 @@
         <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="1">
         <v>0.9</v>
@@ -1186,8 +1245,11 @@
         <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -1195,37 +1257,40 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="D14" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H14" s="1">
         <v>0.1</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="2">
         <v>8</v>
@@ -1234,10 +1299,10 @@
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H15" s="1">
         <v>0.1</v>
@@ -1246,8 +1311,11 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1264,10 +1332,10 @@
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1">
         <v>0.1</v>
@@ -1276,8 +1344,11 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -1294,7 +1365,7 @@
         <v>48</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>62</v>
@@ -1306,8 +1377,11 @@
         <f t="shared" si="0"/>
         <v>18.600000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -1324,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H18" s="1">
         <v>0.1</v>
@@ -1336,8 +1410,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -1351,13 +1428,13 @@
         <v>4</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H19" s="1">
         <v>38.29</v>
@@ -1366,8 +1443,11 @@
         <f t="shared" si="0"/>
         <v>153.16</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
@@ -1384,10 +1464,10 @@
         <v>55</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="H20" s="1">
         <v>2.35</v>
@@ -1396,8 +1476,11 @@
         <f t="shared" si="0"/>
         <v>2.35</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
@@ -1411,10 +1494,10 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>61</v>
@@ -1426,13 +1509,16 @@
         <f t="shared" si="0"/>
         <v>5.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
@@ -1441,13 +1527,13 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H22" s="1">
         <v>0.1</v>
@@ -1456,13 +1542,16 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -1471,13 +1560,13 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="H23" s="1">
         <v>0.1</v>
@@ -1487,12 +1576,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
@@ -1501,13 +1590,13 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H24" s="1">
         <v>0.1</v>
@@ -1516,28 +1605,31 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="2">
         <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H25" s="1">
         <v>0.1</v>
@@ -1546,28 +1638,31 @@
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -1577,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
@@ -1594,10 +1689,10 @@
         <v>17</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H27" s="1">
         <v>0.38</v>
@@ -1606,23 +1701,26 @@
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H29" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I29" s="1">
         <f>SUM(I2:I27)</f>
-        <v>218.36999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>217.56999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H31" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I31" s="1">
         <f>SUM(I8:I27,I2:I6)-H5</f>
-        <v>211.42999999999998</v>
+        <v>210.63</v>
       </c>
     </row>
   </sheetData>
@@ -1633,14 +1731,136 @@
     <hyperlink ref="G11" r:id="rId4" xr:uid="{BB89C172-712E-40A9-BDCE-7E38DB56CE35}"/>
     <hyperlink ref="G17" r:id="rId5" xr:uid="{DAD95586-2E9B-401F-982E-BDF8311324BD}"/>
     <hyperlink ref="G18" r:id="rId6" xr:uid="{9369E23B-C789-4591-B950-41B42E47C50B}"/>
-    <hyperlink ref="G20" r:id="rId7" xr:uid="{86B95A12-F55E-4AD6-9D87-6F657F1E1AEA}"/>
-    <hyperlink ref="G21" r:id="rId8" xr:uid="{EF87F492-CF53-47AE-B507-F3C950142DEA}"/>
-    <hyperlink ref="G3" r:id="rId9" xr:uid="{CDD5D00D-4B98-4A17-BCD1-32BC93136CA6}"/>
-    <hyperlink ref="G6" r:id="rId10" xr:uid="{32880111-13E6-4203-B63A-35EF27715038}"/>
-    <hyperlink ref="G9" r:id="rId11" xr:uid="{C92AB5C7-03AA-44B1-8249-ED2336213ECF}"/>
-    <hyperlink ref="G15" r:id="rId12" xr:uid="{894D25D2-515B-44E2-B238-ECED31845139}"/>
+    <hyperlink ref="G21" r:id="rId7" xr:uid="{EF87F492-CF53-47AE-B507-F3C950142DEA}"/>
+    <hyperlink ref="G3" r:id="rId8" xr:uid="{CDD5D00D-4B98-4A17-BCD1-32BC93136CA6}"/>
+    <hyperlink ref="G6" r:id="rId9" xr:uid="{32880111-13E6-4203-B63A-35EF27715038}"/>
+    <hyperlink ref="G9" r:id="rId10" xr:uid="{C92AB5C7-03AA-44B1-8249-ED2336213ECF}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{894D25D2-515B-44E2-B238-ECED31845139}"/>
+    <hyperlink ref="G4" r:id="rId12" xr:uid="{BB9AFC41-1BE6-4E3A-978F-7C89F10FD15A}"/>
+    <hyperlink ref="G8" r:id="rId13" xr:uid="{EABB31F8-F8A8-44AB-9533-13F7F5263E33}"/>
+    <hyperlink ref="G10" r:id="rId14" xr:uid="{6ED37A7D-F34F-437F-96C1-BB566C2F7271}"/>
+    <hyperlink ref="G12" r:id="rId15" xr:uid="{3DB81C4A-0E4C-4DB3-AFDF-4877A9D65553}"/>
+    <hyperlink ref="G14" r:id="rId16" xr:uid="{65E6814F-D4C4-40C5-97A9-E8FD3240731B}"/>
+    <hyperlink ref="G16" r:id="rId17" xr:uid="{40780725-415E-4AA0-9F9B-B3B53F56972C}"/>
+    <hyperlink ref="G7" r:id="rId18" xr:uid="{E4CC06B0-586E-47F0-BDD3-2C652E3B90A2}"/>
+    <hyperlink ref="G19" r:id="rId19" xr:uid="{3528CB7F-615E-474F-B757-1400A046C3DE}"/>
+    <hyperlink ref="G20" r:id="rId20" xr:uid="{566FD5B3-516D-4722-82B7-CA09303F57C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49472363-7EB1-43C4-8174-BE06D3190168}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="1">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="1">
+        <v>153.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="1">
+        <f>SUM(B2:B9)</f>
+        <v>217.57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Printed out schematic and layout pdfs, fixed BOM
</commit_message>
<xml_diff>
--- a/EECS430W24_Group7_PCB_BOM.xlsx
+++ b/EECS430W24_Group7_PCB_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Desktop\UMich\Class Files\9 2024 Winter\EECS 430\Project\eecs430-phased-array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE9A480-B7E1-4A82-8830-10CBCCFF3547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190D4D73-F55B-4CA7-A56E-4D2F33E3636D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="143">
   <si>
     <t>Quantity</t>
   </si>
@@ -105,9 +105,6 @@
     <t>LED GREEN CLEAR CHIP SMD</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4</t>
-  </si>
-  <si>
     <t>SMA Connector Jack, Female Socket 50 Ohms Board Edge, End Launch Solder</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Red PC Test Point, Miniature Phosphor Bronze Silver Plating Through Hole Mounting Type</t>
   </si>
   <si>
-    <t>TP1.1, TP1.2, TP2.1, TP2.2, TP3.1, TP3.2, TP4.1, TP4.2, TP5.1, TP5.2, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18</t>
-  </si>
-  <si>
     <t>Keystone Electronics</t>
   </si>
   <si>
@@ -429,9 +423,6 @@
     <t>Populated</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>SMA Connectors</t>
   </si>
   <si>
@@ -466,6 +457,15 @@
   </si>
   <si>
     <t>Components</t>
+  </si>
+  <si>
+    <t>D1, D2, D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18</t>
   </si>
 </sst>
 </file>
@@ -822,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,34 +844,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -879,52 +879,52 @@
         <v>5000</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="2">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="2">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1">
         <v>0.38</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I27" si="0">H2*D2</f>
-        <v>8.74</v>
+        <f t="shared" ref="I2:I28" si="0">H2*D2</f>
+        <v>4.9400000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" s="1">
         <v>1.08</v>
@@ -936,25 +936,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H4" s="1">
         <v>1.23</v>
@@ -966,25 +966,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="2">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H5" s="1">
         <v>3.99</v>
@@ -996,25 +996,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H6" s="1">
         <v>0.75</v>
@@ -1026,25 +1026,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
         <v>98</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H7" s="1">
         <v>2.95</v>
@@ -1056,79 +1056,75 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="D8" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H8" s="1">
         <v>0.39</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>1.56</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>1.17</v>
+      </c>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="D9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="H9" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
         <v>107</v>
       </c>
-      <c r="B10" t="s">
-        <v>108</v>
-      </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2">
         <v>3</v>
@@ -1137,436 +1133,412 @@
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H10" s="1">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>0.33</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>84</v>
+        <v>63</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="H11" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-      <c r="I11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.33</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="H12" s="1">
-        <v>1.18</v>
+        <v>0.33</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>2.36</v>
-      </c>
+        <v>0.33</v>
+      </c>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="H13" s="1">
-        <v>0.9</v>
+        <v>1.18</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>130</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="H14" s="1">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>2.7</v>
+      </c>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>111</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="D15" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="H15" s="1">
         <v>0.1</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="H16" s="1">
         <v>0.1</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>0.8</v>
+      </c>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H17" s="1">
-        <v>18.600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="0"/>
-        <v>18.600000000000001</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="H18" s="1">
-        <v>0.1</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="H19" s="1">
-        <v>38.29</v>
+        <v>0.1</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="0"/>
-        <v>153.16</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="H20" s="1">
-        <v>2.35</v>
+        <v>38.29</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
-        <v>2.35</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>153.16</v>
+      </c>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="H21" s="1">
-        <v>5.25</v>
+        <v>2.35</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="0"/>
-        <v>5.25</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>2.35</v>
+      </c>
+      <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="H22" s="1">
-        <v>0.1</v>
+        <v>5.25</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>5.25</v>
+      </c>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="2">
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H23" s="1">
         <v>0.1</v>
@@ -1575,28 +1547,29 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="H24" s="1">
         <v>0.1</v>
@@ -1605,146 +1578,170 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="D25" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H25" s="1">
         <v>0.1</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" t="s">
-        <v>88</v>
+        <v>63</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="1">
         <v>0.38</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I28" s="1">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="1">
-        <f>SUM(I2:I27)</f>
-        <v>217.56999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I31" s="1">
-        <f>SUM(I8:I27,I2:I6)-H5</f>
-        <v>210.63</v>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I30" s="1">
+        <f>SUM(I2:I28)</f>
+        <v>213.37999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H32" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I32" s="1">
+        <f>SUM(I8:I28,I2:I6)-H5</f>
+        <v>206.43999999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{E088431F-7E54-4277-94E0-EA1C4CFA4751}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{2B8D2EB7-258A-4968-88D1-7D47CF687E63}"/>
-    <hyperlink ref="G13" r:id="rId3" xr:uid="{A4D04541-F2EE-43A5-9B6F-381295AD7F2E}"/>
-    <hyperlink ref="G11" r:id="rId4" xr:uid="{BB89C172-712E-40A9-BDCE-7E38DB56CE35}"/>
-    <hyperlink ref="G17" r:id="rId5" xr:uid="{DAD95586-2E9B-401F-982E-BDF8311324BD}"/>
-    <hyperlink ref="G18" r:id="rId6" xr:uid="{9369E23B-C789-4591-B950-41B42E47C50B}"/>
-    <hyperlink ref="G21" r:id="rId7" xr:uid="{EF87F492-CF53-47AE-B507-F3C950142DEA}"/>
+    <hyperlink ref="G14" r:id="rId3" xr:uid="{A4D04541-F2EE-43A5-9B6F-381295AD7F2E}"/>
+    <hyperlink ref="G12" r:id="rId4" xr:uid="{BB89C172-712E-40A9-BDCE-7E38DB56CE35}"/>
+    <hyperlink ref="G18" r:id="rId5" xr:uid="{DAD95586-2E9B-401F-982E-BDF8311324BD}"/>
+    <hyperlink ref="G19" r:id="rId6" xr:uid="{9369E23B-C789-4591-B950-41B42E47C50B}"/>
+    <hyperlink ref="G22" r:id="rId7" xr:uid="{EF87F492-CF53-47AE-B507-F3C950142DEA}"/>
     <hyperlink ref="G3" r:id="rId8" xr:uid="{CDD5D00D-4B98-4A17-BCD1-32BC93136CA6}"/>
     <hyperlink ref="G6" r:id="rId9" xr:uid="{32880111-13E6-4203-B63A-35EF27715038}"/>
-    <hyperlink ref="G9" r:id="rId10" xr:uid="{C92AB5C7-03AA-44B1-8249-ED2336213ECF}"/>
-    <hyperlink ref="G15" r:id="rId11" xr:uid="{894D25D2-515B-44E2-B238-ECED31845139}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{C92AB5C7-03AA-44B1-8249-ED2336213ECF}"/>
+    <hyperlink ref="G16" r:id="rId11" xr:uid="{894D25D2-515B-44E2-B238-ECED31845139}"/>
     <hyperlink ref="G4" r:id="rId12" xr:uid="{BB9AFC41-1BE6-4E3A-978F-7C89F10FD15A}"/>
     <hyperlink ref="G8" r:id="rId13" xr:uid="{EABB31F8-F8A8-44AB-9533-13F7F5263E33}"/>
-    <hyperlink ref="G10" r:id="rId14" xr:uid="{6ED37A7D-F34F-437F-96C1-BB566C2F7271}"/>
-    <hyperlink ref="G12" r:id="rId15" xr:uid="{3DB81C4A-0E4C-4DB3-AFDF-4877A9D65553}"/>
-    <hyperlink ref="G14" r:id="rId16" xr:uid="{65E6814F-D4C4-40C5-97A9-E8FD3240731B}"/>
-    <hyperlink ref="G16" r:id="rId17" xr:uid="{40780725-415E-4AA0-9F9B-B3B53F56972C}"/>
+    <hyperlink ref="G11" r:id="rId14" xr:uid="{6ED37A7D-F34F-437F-96C1-BB566C2F7271}"/>
+    <hyperlink ref="G13" r:id="rId15" xr:uid="{3DB81C4A-0E4C-4DB3-AFDF-4877A9D65553}"/>
+    <hyperlink ref="G15" r:id="rId16" xr:uid="{65E6814F-D4C4-40C5-97A9-E8FD3240731B}"/>
+    <hyperlink ref="G17" r:id="rId17" xr:uid="{40780725-415E-4AA0-9F9B-B3B53F56972C}"/>
     <hyperlink ref="G7" r:id="rId18" xr:uid="{E4CC06B0-586E-47F0-BDD3-2C652E3B90A2}"/>
-    <hyperlink ref="G19" r:id="rId19" xr:uid="{3528CB7F-615E-474F-B757-1400A046C3DE}"/>
-    <hyperlink ref="G20" r:id="rId20" xr:uid="{566FD5B3-516D-4722-82B7-CA09303F57C7}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{3528CB7F-615E-474F-B757-1400A046C3DE}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{566FD5B3-516D-4722-82B7-CA09303F57C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>
@@ -1767,15 +1764,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1">
         <v>11.97</v>
@@ -1783,7 +1780,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1">
         <v>3.54</v>
@@ -1791,7 +1788,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1">
         <v>3.7</v>
@@ -1799,7 +1796,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B5" s="1">
         <v>18.600000000000001</v>
@@ -1807,7 +1804,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B6" s="1">
         <v>153.16</v>
@@ -1815,7 +1812,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B7" s="1">
         <v>2.35</v>
@@ -1823,7 +1820,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B8" s="1">
         <v>5.25</v>
@@ -1831,7 +1828,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="1">
         <v>19</v>
@@ -1839,7 +1836,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" s="1">
         <f>SUM(B2:B9)</f>
@@ -1848,15 +1845,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switched phase shifter link to digikey
</commit_message>
<xml_diff>
--- a/EECS430W24_Group7_PCB_BOM.xlsx
+++ b/EECS430W24_Group7_PCB_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Desktop\UMich\Class Files\9 2024 Winter\EECS 430\Project\eecs430-phased-array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190D4D73-F55B-4CA7-A56E-4D2F33E3636D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1BE020-1600-43BC-9CEA-E439579D6364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,9 +339,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/MACOM/MAPS-010145-TR0500?qs=gRMouoDVsgLV0nPQKDDWAA%3D%3D</t>
-  </si>
-  <si>
     <t>MACOM</t>
   </si>
   <si>
@@ -466,6 +463,9 @@
   </si>
   <si>
     <t>TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/macom-technology-solutions/MAPS-010145-TR0500/4429760?s=N4IgTCBcDaILIEEAKBlAtABgIzYCwFY0AVAJQ3wwxAF0BfIA</t>
   </si>
 </sst>
 </file>
@@ -825,7 +825,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,7 +871,7 @@
         <v>76</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -882,7 +882,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D2" s="2">
         <v>13</v>
@@ -1062,7 +1062,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -1090,10 +1090,10 @@
         <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -1104,7 +1104,7 @@
       <c r="F9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>86</v>
       </c>
       <c r="H9" s="1">
@@ -1118,10 +1118,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1136,7 +1136,7 @@
         <v>63</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" s="1">
         <v>0.1</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
         <v>105</v>
-      </c>
-      <c r="B11" t="s">
-        <v>106</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1167,7 +1167,7 @@
         <v>63</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" s="1">
         <v>0.11</v>
@@ -1278,7 +1278,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
         <v>78</v>
@@ -1321,7 +1321,7 @@
         <v>63</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H16" s="1">
         <v>0.1</v>
@@ -1439,20 +1439,20 @@
         <v>4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="H20" s="1">
-        <v>38.29</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
-        <v>153.16</v>
+        <v>154.80000000000001</v>
       </c>
       <c r="J20" s="1"/>
     </row>
@@ -1476,7 +1476,7 @@
         <v>61</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H21" s="1">
         <v>2.35</v>
@@ -1520,10 +1520,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
         <v>110</v>
-      </c>
-      <c r="B23" t="s">
-        <v>111</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -1532,13 +1532,13 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="H23" s="1">
         <v>0.1</v>
@@ -1551,10 +1551,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
@@ -1563,13 +1563,13 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H24" s="1">
         <v>0.1</v>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" t="s">
         <v>118</v>
-      </c>
-      <c r="B25" t="s">
-        <v>119</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -1593,13 +1593,13 @@
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H25" s="1">
         <v>0.1</v>
@@ -1612,10 +1612,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" t="s">
         <v>121</v>
-      </c>
-      <c r="B26" t="s">
-        <v>122</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -1624,13 +1624,13 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H26" s="1">
         <v>0.1</v>
@@ -1646,7 +1646,7 @@
         <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
         <v>72</v>
@@ -1708,16 +1708,16 @@
       </c>
       <c r="I30" s="1">
         <f>SUM(I2:I28)</f>
-        <v>213.37999999999997</v>
+        <v>215.01999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H32" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I32" s="1">
         <f>SUM(I8:I28,I2:I6)-H5</f>
-        <v>206.43999999999997</v>
+        <v>208.07999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1764,15 +1764,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
         <v>136</v>
-      </c>
-      <c r="B1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1">
         <v>11.97</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="1">
         <v>3.54</v>
@@ -1788,7 +1788,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="1">
         <v>3.7</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1">
         <v>18.600000000000001</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="1">
         <v>153.16</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" s="1">
         <v>2.35</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="1">
         <v>5.25</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="1">
         <v>19</v>
@@ -1845,15 +1845,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>